<commit_message>
Added some more images, reworked some texts
</commit_message>
<xml_diff>
--- a/assets/files/examples/Peakboard_Example_Date.xlsx
+++ b/assets/files/examples/Peakboard_Example_Date.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/Desktop/temp/Get_Started_Help/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/git/peakboard-help/assets/files/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F8F0925-7CA9-6743-AA92-78D1C91ED097}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4778281-CB82-4B47-8DCE-B8EA3845669A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{792B7A18-EF4F-C84E-BCF9-07BEB9C7F81B}"/>
   </bookViews>
@@ -431,7 +431,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -461,7 +461,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="1">
-        <v>437</v>
+        <v>4678</v>
       </c>
       <c r="D2" s="1">
         <v>500</v>
@@ -495,7 +495,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="1">
-        <v>1399</v>
+        <v>699</v>
       </c>
       <c r="D4" s="1">
         <v>800</v>

</xml_diff>